<commit_message>
added benchmark index calculation, and daily plotting function with combined notional volume
</commit_message>
<xml_diff>
--- a/processed_vol_trend_data_long/pivots_long.xlsx
+++ b/processed_vol_trend_data_long/pivots_long.xlsx
@@ -823,28 +823,28 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C18" t="n">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="D18" t="n">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="E18" t="n">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="F18" t="n">
-        <v>39</v>
+        <v>86</v>
       </c>
       <c r="G18" t="n">
         <v>116</v>
       </c>
       <c r="H18" t="n">
-        <v>485</v>
+        <v>511</v>
       </c>
       <c r="I18" t="n">
-        <v>31.14964675658317</v>
+        <v>32.67263427109975</v>
       </c>
     </row>
     <row r="19">
@@ -854,28 +854,28 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D19" t="n">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="E19" t="n">
-        <v>81</v>
+        <v>37</v>
       </c>
       <c r="F19" t="n">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="G19" t="n">
         <v>87</v>
       </c>
       <c r="H19" t="n">
-        <v>290</v>
+        <v>257</v>
       </c>
       <c r="I19" t="n">
-        <v>18.62556197816313</v>
+        <v>16.43222506393862</v>
       </c>
     </row>
     <row r="20">
@@ -885,28 +885,28 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="C20" t="n">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="D20" t="n">
-        <v>86</v>
+        <v>122</v>
       </c>
       <c r="E20" t="n">
-        <v>39</v>
+        <v>108</v>
       </c>
       <c r="F20" t="n">
-        <v>142</v>
+        <v>95</v>
       </c>
       <c r="G20" t="n">
         <v>33</v>
       </c>
       <c r="H20" t="n">
-        <v>505</v>
+        <v>582</v>
       </c>
       <c r="I20" t="n">
-        <v>32.43416827231856</v>
+        <v>37.21227621483376</v>
       </c>
     </row>
     <row r="21">
@@ -919,25 +919,25 @@
         <v>53</v>
       </c>
       <c r="C21" t="n">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="D21" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E21" t="n">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="F21" t="n">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="G21" t="n">
         <v>26</v>
       </c>
       <c r="H21" t="n">
-        <v>277</v>
+        <v>214</v>
       </c>
       <c r="I21" t="n">
-        <v>17.79062299293513</v>
+        <v>13.68286445012788</v>
       </c>
     </row>
     <row r="22">
@@ -991,28 +991,28 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C25" t="n">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="D25" t="n">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="E25" t="n">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="F25" t="n">
-        <v>121</v>
+        <v>64</v>
       </c>
       <c r="G25" t="n">
-        <v>98</v>
+        <v>140</v>
       </c>
       <c r="H25" t="n">
-        <v>528</v>
+        <v>534</v>
       </c>
       <c r="I25" t="n">
-        <v>33.97683397683397</v>
+        <v>32.88177339901478</v>
       </c>
     </row>
     <row r="26">
@@ -1022,28 +1022,28 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C26" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D26" t="n">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="E26" t="n">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="F26" t="n">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="G26" t="n">
         <v>54</v>
       </c>
       <c r="H26" t="n">
-        <v>250</v>
+        <v>283</v>
       </c>
       <c r="I26" t="n">
-        <v>16.08751608751609</v>
+        <v>17.42610837438423</v>
       </c>
     </row>
     <row r="27">
@@ -1053,28 +1053,28 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="C27" t="n">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D27" t="n">
-        <v>122</v>
+        <v>86</v>
       </c>
       <c r="E27" t="n">
-        <v>108</v>
+        <v>39</v>
       </c>
       <c r="F27" t="n">
-        <v>54</v>
+        <v>111</v>
       </c>
       <c r="G27" t="n">
-        <v>69</v>
+        <v>104</v>
       </c>
       <c r="H27" t="n">
-        <v>577</v>
+        <v>545</v>
       </c>
       <c r="I27" t="n">
-        <v>37.12998712998713</v>
+        <v>33.55911330049261</v>
       </c>
     </row>
     <row r="28">
@@ -1087,25 +1087,25 @@
         <v>53</v>
       </c>
       <c r="C28" t="n">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="D28" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E28" t="n">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="F28" t="n">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="G28" t="n">
         <v>36</v>
       </c>
       <c r="H28" t="n">
-        <v>199</v>
+        <v>262</v>
       </c>
       <c r="I28" t="n">
-        <v>12.80566280566281</v>
+        <v>16.13300492610837</v>
       </c>
     </row>
   </sheetData>

</xml_diff>